<commit_message>
PC naar laptop update
</commit_message>
<xml_diff>
--- a/documentatie/B1-K2/W1/stage logboek.xlsx
+++ b/documentatie/B1-K2/W1/stage logboek.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>BPV-logboek</t>
   </si>
@@ -322,6 +322,21 @@
   <si>
     <t>Functioneel comentaar toegevoegd aan alle code
 Evaluatie verslag geschreven</t>
+  </si>
+  <si>
+    <t>Bugs oplossen en bestand erover gemaakt.
+Bugs bedacht voor stan en die in mijn systeem neer gezet zodat hij die kan oplossen</t>
+  </si>
+  <si>
+    <t>To Fo aangepast en aanpasdocument gemaakt</t>
+  </si>
+  <si>
+    <t>Gegevens beheren document gemaakt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evalutie verslage aangepast naar wensen Arno
+Handtekeningen onder Testrapporten en evaluatie verslag gekregen
+</t>
   </si>
   <si>
     <t>Totaal aantal uren:</t>
@@ -4181,10 +4196,10 @@
       <c r="C85" s="25">
         <v>43971.0</v>
       </c>
-      <c r="D85" s="35" t="s">
+      <c r="D85" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="E85" s="36">
+      <c r="E85" s="32">
         <v>8.5</v>
       </c>
       <c r="F85" s="6"/>
@@ -4219,8 +4234,12 @@
       <c r="C86" s="25">
         <v>43972.0</v>
       </c>
-      <c r="D86" s="34"/>
-      <c r="E86" s="32"/>
+      <c r="D86" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="E86" s="32">
+        <v>8.5</v>
+      </c>
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
       <c r="H86" s="6"/>
@@ -4253,8 +4272,12 @@
       <c r="C87" s="25">
         <v>43973.0</v>
       </c>
-      <c r="D87" s="34"/>
-      <c r="E87" s="32"/>
+      <c r="D87" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E87" s="32">
+        <v>16.5</v>
+      </c>
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
       <c r="H87" s="6"/>
@@ -4287,8 +4310,12 @@
       <c r="C88" s="25">
         <v>43976.0</v>
       </c>
-      <c r="D88" s="34"/>
-      <c r="E88" s="32"/>
+      <c r="D88" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E88" s="32">
+        <v>8.5</v>
+      </c>
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
       <c r="H88" s="6"/>
@@ -4321,8 +4348,12 @@
       <c r="C89" s="25">
         <v>43977.0</v>
       </c>
-      <c r="D89" s="34"/>
-      <c r="E89" s="32"/>
+      <c r="D89" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="E89" s="36">
+        <v>8.5</v>
+      </c>
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
       <c r="H89" s="6"/>
@@ -5234,12 +5265,12 @@
       <c r="B116" s="43"/>
       <c r="C116" s="9"/>
       <c r="D116" s="26" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E116" s="24">
         <f>sum(E8+E9+E10+E11+E12+E13+E14+E15+E16+E17+E18+E19+E20+E21+E22+E23+E24+E25+E26+E27+E28+E29+E30+E31+E32+E33+E34+E35+E36+E37+E38+E39+E40+E41+E42+E43+E44+E45+E46+E47+E48+E49+E50+E51+E52+E53+E54+E55+E56+E57+E58+E59+E60+E61+E62+E63+E64+E65+E66+E67+E68+E69+E70+E71+E72+E73+E74+E75+E76+E77+E78+E79+E80+E81+E82+E83+E84+E85+E86+E87+E88+E89+E90+E91+E92+E93+E94+E95+E96+E97+E98+E99+E100+E101+E102+E103+E104+E105+E106+E107+E108+E109+E110+E111+E112+E113+E114+E115
 )</f>
-        <v>555</v>
+        <v>597</v>
       </c>
       <c r="F116" s="16"/>
       <c r="G116" s="6"/>
@@ -5268,7 +5299,7 @@
       <c r="B117" s="8"/>
       <c r="C117" s="11"/>
       <c r="D117" s="26" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E117" s="24">
         <v>704.0</v>
@@ -5300,11 +5331,11 @@
       <c r="B118" s="8"/>
       <c r="C118" s="11"/>
       <c r="D118" s="26" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E118" s="24">
         <f>SUM(E117-E116)</f>
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="F118" s="44"/>
       <c r="G118" s="44"/>
@@ -5333,7 +5364,7 @@
       <c r="B119" s="8"/>
       <c r="C119" s="11"/>
       <c r="D119" s="26" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E119" s="24">
         <f>SUM(B115-(E117/40))</f>
@@ -5372,13 +5403,13 @@
       <c r="B120" s="8"/>
       <c r="C120" s="11"/>
       <c r="D120" s="46" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E120" s="38">
         <v>0.0</v>
       </c>
       <c r="F120" s="47" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G120" s="48">
         <f>SUM(F119-E120)</f>

</xml_diff>